<commit_message>
Add steps for masting Calculator magic and fix sorting
</commit_message>
<xml_diff>
--- a/Assets/Exports/Main Characters.xlsx
+++ b/Assets/Exports/Main Characters.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="114">
   <si>
     <t>Ramza</t>
   </si>
@@ -166,30 +166,45 @@
     <t>Move-MP Up</t>
   </si>
   <si>
+    <t>Gained JP Up: (Squire - 250 JP)</t>
+  </si>
+  <si>
+    <t>Move +1: (Squire - 200 JP)</t>
+  </si>
+  <si>
     <t>2 Squire</t>
   </si>
   <si>
+    <t>Auto Potion: (Chemist - 400 JP)</t>
+  </si>
+  <si>
+    <t>2 Chemist</t>
+  </si>
+  <si>
+    <t>Master Chemist! (4,040 JP)</t>
+  </si>
+  <si>
+    <t>Speed Save: (Archer - 800 JP)</t>
+  </si>
+  <si>
+    <t>Master Priest! (5,510 JP)</t>
+  </si>
+  <si>
+    <t>3 Archer</t>
+  </si>
+  <si>
+    <t>3 Knight</t>
+  </si>
+  <si>
     <t>Master Engineer! (700 JP)</t>
   </si>
   <si>
-    <t>Master Chemist! (4,040 JP)</t>
-  </si>
-  <si>
     <t>Master Heaven Knight! (2,000 JP)</t>
   </si>
   <si>
-    <t>2 Chemist</t>
-  </si>
-  <si>
-    <t>3 Knight</t>
-  </si>
-  <si>
     <t>2 Knight</t>
   </si>
   <si>
-    <t>Speed Save: (Archer - 800 JP)</t>
-  </si>
-  <si>
     <t>4 Priest</t>
   </si>
   <si>
@@ -199,7 +214,7 @@
     <t>Master Knight! (2,400 JP)</t>
   </si>
   <si>
-    <t>3 Archer</t>
+    <t>Move +2: (Thief - 520 JP)</t>
   </si>
   <si>
     <t>2 Wizard</t>
@@ -217,13 +232,16 @@
     <t>Master Monk! (2,700 JP)</t>
   </si>
   <si>
+    <t>Master Wizard! (6,890 JP)</t>
+  </si>
+  <si>
     <t>Master Thief! (2,660 JP)</t>
   </si>
   <si>
     <t>Concentrate: (Archer - 400 JP)</t>
   </si>
   <si>
-    <t>Move +2: (Thief - 520 JP)</t>
+    <t>4 Thief</t>
   </si>
   <si>
     <t>Short Charge: (Time Mage - 800 JP)</t>
@@ -238,97 +256,97 @@
     <t>Master Geomancer! (1,800 JP)</t>
   </si>
   <si>
+    <t>Master Lancer! (5,400 JP)</t>
+  </si>
+  <si>
+    <t>2 Time Mage</t>
+  </si>
+  <si>
+    <t>2 Thief</t>
+  </si>
+  <si>
+    <t>Attack Up: (Geomancer - 400 JP)</t>
+  </si>
+  <si>
     <t>4 Wizard</t>
   </si>
   <si>
-    <t>4 Thief</t>
-  </si>
-  <si>
-    <t>2 Time Mage</t>
-  </si>
-  <si>
-    <t>2 Thief</t>
-  </si>
-  <si>
-    <t>Attack Up: (Geomancer - 400 JP)</t>
+    <t>Master Summoner! (7,950 JP)</t>
+  </si>
+  <si>
+    <t>2 Lancer</t>
+  </si>
+  <si>
+    <t>Master Time Mage! (5,300 JP)</t>
   </si>
   <si>
     <t>MP Switch: (Time Mage - 400 JP)</t>
   </si>
   <si>
-    <t>Master Lancer! (5,400 JP)</t>
-  </si>
-  <si>
-    <t>Master Summoner! (7,950 JP)</t>
-  </si>
-  <si>
-    <t>2 Lancer</t>
+    <t>Counter: (Monk - 300 JP)</t>
+  </si>
+  <si>
+    <t>Master Samurai! (4,600 JP)</t>
+  </si>
+  <si>
+    <t>2 Geomancer</t>
+  </si>
+  <si>
+    <t>Blade Grasp: (Samurai - 700 JP)</t>
   </si>
   <si>
     <t>3 Time Mage</t>
   </si>
   <si>
-    <t>Master Samurai! (4,600 JP)</t>
+    <t>Master Ninja! (1,120 JP)</t>
   </si>
   <si>
     <t>Move-MP Up: (Oracle - 350 JP)</t>
   </si>
   <si>
-    <t>Counter: (Monk - 300 JP)</t>
-  </si>
-  <si>
-    <t>2 Geomancer</t>
-  </si>
-  <si>
-    <t>Blade Grasp: (Samurai - 700 JP)</t>
+    <t>4 Summoner</t>
+  </si>
+  <si>
+    <t>Two Swords: (Ninja - 900 JP)</t>
   </si>
   <si>
     <t>3 Oracle</t>
   </si>
   <si>
-    <t>Two Swords: (Ninja - 900 JP)</t>
-  </si>
-  <si>
-    <t>Master Ninja! (1,120 JP)</t>
+    <t>Master Oracle! (4,670 JP)</t>
+  </si>
+  <si>
+    <t>Master Soldier! (4,380 JP)</t>
+  </si>
+  <si>
+    <t>Damage Split: (Calculator - 300 JP)</t>
+  </si>
+  <si>
+    <t>Master Divine Knight! (1,900 JP)</t>
+  </si>
+  <si>
+    <t>2 Oracle</t>
+  </si>
+  <si>
+    <t>Teleport: (Time Mage - 600 JP)</t>
+  </si>
+  <si>
+    <t>4 Mediator</t>
+  </si>
+  <si>
+    <t>Master Holy Knight! (2,500 JP)</t>
+  </si>
+  <si>
+    <t>Master Temple Knight! (3,290 JP)</t>
   </si>
   <si>
     <t>Master Calculator! (2,550 JP)</t>
   </si>
   <si>
-    <t>4 Summoner</t>
+    <t>Move +3: (Bard - 1,000 JP)</t>
   </si>
   <si>
     <t>Master Dragoner! (2,300 JP)</t>
-  </si>
-  <si>
-    <t>Master Soldier! (4,380 JP)</t>
-  </si>
-  <si>
-    <t>Master Time Mage! (5,300 JP)</t>
-  </si>
-  <si>
-    <t>Damage Split: (Calculator - 300 JP)</t>
-  </si>
-  <si>
-    <t>Master Divine Knight! (1,900 JP)</t>
-  </si>
-  <si>
-    <t>2 Oracle</t>
-  </si>
-  <si>
-    <t>Teleport: (Time Mage - 600 JP)</t>
-  </si>
-  <si>
-    <t>4 Mediator</t>
-  </si>
-  <si>
-    <t>Master Holy Knight! (2,500 JP)</t>
-  </si>
-  <si>
-    <t>Master Temple Knight! (3,290 JP)</t>
-  </si>
-  <si>
-    <t>Move +3: (Bard - 1,000 JP)</t>
   </si>
   <si>
     <t>Master Mediator! (2,200 JP)</t>
@@ -702,7 +720,7 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:N26"/>
+  <dimension ref="A1:N29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" topLeftCell="A1" zoomScaleNormal="100" zoomScaleSheetLayoutView="60" zoomScale="100" view="normal"/>
   </sheetViews>
@@ -965,19 +983,19 @@
         <v>0</v>
       </c>
       <c r="E9" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="G9" s="2" t="b">
         <v>0</v>
       </c>
       <c r="H9" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="J9" s="2" t="b">
         <v>0</v>
       </c>
       <c r="K9" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="M9" s="2" t="b">
         <v>0</v>
@@ -1007,7 +1025,7 @@
         <v>0</v>
       </c>
       <c r="Z9" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="AB9" s="2" t="b">
         <v>0</v>
@@ -1031,7 +1049,7 @@
         <v>0</v>
       </c>
       <c r="AL9" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
     </row>
     <row r="10">
@@ -1039,79 +1057,79 @@
         <v>0</v>
       </c>
       <c r="B10" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="D10" s="2" t="b">
         <v>0</v>
       </c>
       <c r="E10" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="G10" s="2" t="b">
         <v>0</v>
       </c>
       <c r="H10" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="J10" s="2" t="b">
         <v>0</v>
       </c>
       <c r="K10" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="M10" s="2" t="b">
         <v>0</v>
       </c>
       <c r="N10" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="P10" s="2" t="b">
         <v>0</v>
       </c>
       <c r="Q10" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="S10" s="2" t="b">
         <v>0</v>
       </c>
       <c r="T10" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="V10" s="2" t="b">
         <v>0</v>
       </c>
       <c r="W10" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="Y10" s="2" t="b">
         <v>0</v>
       </c>
       <c r="Z10" t="s">
-        <v>58</v>
+        <v>51</v>
       </c>
       <c r="AB10" s="2" t="b">
         <v>0</v>
       </c>
       <c r="AC10" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="AE10" s="2" t="b">
         <v>0</v>
       </c>
       <c r="AF10" t="s">
-        <v>60</v>
+        <v>51</v>
       </c>
       <c r="AH10" s="2" t="b">
         <v>0</v>
       </c>
       <c r="AI10" t="s">
-        <v>61</v>
+        <v>51</v>
       </c>
       <c r="AK10" s="2" t="b">
         <v>0</v>
       </c>
       <c r="AL10" t="s">
-        <v>62</v>
+        <v>51</v>
       </c>
     </row>
     <row r="11">
@@ -1119,79 +1137,79 @@
         <v>0</v>
       </c>
       <c r="B11" t="s">
-        <v>63</v>
+        <v>52</v>
       </c>
       <c r="D11" s="2" t="b">
         <v>0</v>
       </c>
       <c r="E11" t="s">
-        <v>64</v>
+        <v>52</v>
       </c>
       <c r="G11" s="2" t="b">
         <v>0</v>
       </c>
       <c r="H11" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="J11" s="2" t="b">
         <v>0</v>
       </c>
       <c r="K11" t="s">
-        <v>65</v>
+        <v>52</v>
       </c>
       <c r="M11" s="2" t="b">
         <v>0</v>
       </c>
       <c r="N11" t="s">
-        <v>63</v>
+        <v>52</v>
       </c>
       <c r="P11" s="2" t="b">
         <v>0</v>
       </c>
       <c r="Q11" t="s">
-        <v>66</v>
+        <v>52</v>
       </c>
       <c r="S11" s="2" t="b">
         <v>0</v>
       </c>
       <c r="T11" t="s">
-        <v>61</v>
+        <v>52</v>
       </c>
       <c r="V11" s="2" t="b">
         <v>0</v>
       </c>
       <c r="W11" t="s">
-        <v>63</v>
+        <v>52</v>
       </c>
       <c r="Y11" s="2" t="b">
         <v>0</v>
       </c>
       <c r="Z11" t="s">
-        <v>65</v>
+        <v>53</v>
       </c>
       <c r="AB11" s="2" t="b">
         <v>0</v>
       </c>
       <c r="AC11" t="s">
-        <v>67</v>
+        <v>52</v>
       </c>
       <c r="AE11" s="2" t="b">
         <v>0</v>
       </c>
       <c r="AF11" t="s">
-        <v>68</v>
+        <v>52</v>
       </c>
       <c r="AH11" s="2" t="b">
         <v>0</v>
       </c>
       <c r="AI11" t="s">
-        <v>69</v>
+        <v>52</v>
       </c>
       <c r="AK11" s="2" t="b">
         <v>0</v>
       </c>
       <c r="AL11" t="s">
-        <v>70</v>
+        <v>52</v>
       </c>
     </row>
     <row r="12">
@@ -1199,79 +1217,79 @@
         <v>0</v>
       </c>
       <c r="B12" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="D12" s="2" t="b">
         <v>0</v>
       </c>
       <c r="E12" t="s">
-        <v>71</v>
+        <v>53</v>
       </c>
       <c r="G12" s="2" t="b">
         <v>0</v>
       </c>
       <c r="H12" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
       <c r="J12" s="2" t="b">
         <v>0</v>
       </c>
       <c r="K12" t="s">
-        <v>62</v>
+        <v>53</v>
       </c>
       <c r="M12" s="2" t="b">
         <v>0</v>
       </c>
       <c r="N12" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="P12" s="2" t="b">
         <v>0</v>
       </c>
       <c r="Q12" t="s">
-        <v>72</v>
+        <v>53</v>
       </c>
       <c r="S12" s="2" t="b">
         <v>0</v>
       </c>
       <c r="T12" t="s">
-        <v>69</v>
+        <v>53</v>
       </c>
       <c r="V12" s="2" t="b">
         <v>0</v>
       </c>
       <c r="W12" t="s">
-        <v>73</v>
+        <v>53</v>
       </c>
       <c r="Y12" s="2" t="b">
         <v>0</v>
       </c>
       <c r="Z12" t="s">
-        <v>74</v>
+        <v>54</v>
       </c>
       <c r="AB12" s="2" t="b">
         <v>0</v>
       </c>
       <c r="AC12" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="AE12" s="2" t="b">
         <v>0</v>
       </c>
       <c r="AF12" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="AH12" s="2" t="b">
         <v>0</v>
       </c>
       <c r="AI12" t="s">
-        <v>75</v>
+        <v>53</v>
       </c>
       <c r="AK12" s="2" t="b">
         <v>0</v>
       </c>
       <c r="AL12" t="s">
-        <v>76</v>
+        <v>53</v>
       </c>
     </row>
     <row r="13">
@@ -1279,43 +1297,43 @@
         <v>0</v>
       </c>
       <c r="B13" t="s">
-        <v>77</v>
+        <v>54</v>
       </c>
       <c r="D13" s="2" t="b">
         <v>0</v>
       </c>
       <c r="E13" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="G13" s="2" t="b">
         <v>0</v>
       </c>
       <c r="H13" t="s">
-        <v>75</v>
+        <v>55</v>
       </c>
       <c r="J13" s="2" t="b">
         <v>0</v>
       </c>
       <c r="K13" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="M13" s="2" t="b">
         <v>0</v>
       </c>
       <c r="N13" t="s">
-        <v>77</v>
+        <v>54</v>
       </c>
       <c r="P13" s="2" t="b">
         <v>0</v>
       </c>
       <c r="Q13" t="s">
-        <v>78</v>
+        <v>54</v>
       </c>
       <c r="S13" s="2" t="b">
         <v>0</v>
       </c>
       <c r="T13" t="s">
-        <v>75</v>
+        <v>56</v>
       </c>
       <c r="V13" s="2" t="b">
         <v>0</v>
@@ -1327,31 +1345,31 @@
         <v>0</v>
       </c>
       <c r="Z13" t="s">
-        <v>79</v>
+        <v>57</v>
       </c>
       <c r="AB13" s="2" t="b">
         <v>0</v>
       </c>
       <c r="AC13" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
       <c r="AE13" s="2" t="b">
         <v>0</v>
       </c>
       <c r="AF13" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="AH13" s="2" t="b">
         <v>0</v>
       </c>
       <c r="AI13" t="s">
-        <v>80</v>
+        <v>58</v>
       </c>
       <c r="AK13" s="2" t="b">
         <v>0</v>
       </c>
       <c r="AL13" t="s">
-        <v>81</v>
+        <v>54</v>
       </c>
     </row>
     <row r="14">
@@ -1359,79 +1377,79 @@
         <v>0</v>
       </c>
       <c r="B14" t="s">
-        <v>82</v>
+        <v>59</v>
       </c>
       <c r="D14" s="2" t="b">
         <v>0</v>
       </c>
       <c r="E14" t="s">
-        <v>55</v>
+        <v>60</v>
       </c>
       <c r="G14" s="2" t="b">
         <v>0</v>
       </c>
       <c r="H14" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="J14" s="2" t="b">
         <v>0</v>
       </c>
       <c r="K14" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="M14" s="2" t="b">
         <v>0</v>
       </c>
       <c r="N14" t="s">
-        <v>82</v>
+        <v>59</v>
       </c>
       <c r="P14" s="2" t="b">
         <v>0</v>
       </c>
       <c r="Q14" t="s">
-        <v>54</v>
+        <v>62</v>
       </c>
       <c r="S14" s="2" t="b">
         <v>0</v>
       </c>
       <c r="T14" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="V14" s="2" t="b">
         <v>0</v>
       </c>
       <c r="W14" t="s">
+        <v>59</v>
+      </c>
+      <c r="Y14" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="Z14" t="s">
+        <v>63</v>
+      </c>
+      <c r="AB14" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="AC14" t="s">
         <v>64</v>
       </c>
-      <c r="Y14" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="Z14" t="s">
-        <v>83</v>
-      </c>
-      <c r="AB14" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="AC14" t="s">
-        <v>70</v>
-      </c>
       <c r="AE14" s="2" t="b">
         <v>0</v>
       </c>
       <c r="AF14" t="s">
-        <v>54</v>
+        <v>65</v>
       </c>
       <c r="AH14" s="2" t="b">
         <v>0</v>
       </c>
       <c r="AI14" t="s">
-        <v>56</v>
+        <v>66</v>
       </c>
       <c r="AK14" s="2" t="b">
         <v>0</v>
       </c>
       <c r="AL14" t="s">
-        <v>50</v>
+        <v>67</v>
       </c>
     </row>
     <row r="15">
@@ -1439,79 +1457,79 @@
         <v>0</v>
       </c>
       <c r="B15" t="s">
-        <v>84</v>
+        <v>68</v>
       </c>
       <c r="D15" s="2" t="b">
         <v>0</v>
       </c>
       <c r="E15" t="s">
-        <v>63</v>
+        <v>69</v>
       </c>
       <c r="G15" s="2" t="b">
         <v>0</v>
       </c>
       <c r="H15" t="s">
+        <v>56</v>
+      </c>
+      <c r="J15" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="K15" t="s">
+        <v>70</v>
+      </c>
+      <c r="M15" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="N15" t="s">
+        <v>68</v>
+      </c>
+      <c r="P15" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q15" t="s">
+        <v>71</v>
+      </c>
+      <c r="S15" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="T15" t="s">
+        <v>66</v>
+      </c>
+      <c r="V15" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="W15" t="s">
+        <v>68</v>
+      </c>
+      <c r="Y15" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="Z15" t="s">
         <v>72</v>
       </c>
-      <c r="J15" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="K15" t="s">
-        <v>63</v>
-      </c>
-      <c r="M15" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="N15" t="s">
-        <v>84</v>
-      </c>
-      <c r="P15" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="Q15" t="s">
-        <v>58</v>
-      </c>
-      <c r="S15" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="T15" t="s">
-        <v>72</v>
-      </c>
-      <c r="V15" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="W15" t="s">
-        <v>71</v>
-      </c>
-      <c r="Y15" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="Z15" t="s">
-        <v>85</v>
-      </c>
       <c r="AB15" s="2" t="b">
         <v>0</v>
       </c>
       <c r="AC15" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="AE15" s="2" t="b">
         <v>0</v>
       </c>
       <c r="AF15" t="s">
-        <v>62</v>
+        <v>74</v>
       </c>
       <c r="AH15" s="2" t="b">
         <v>0</v>
       </c>
       <c r="AI15" t="s">
-        <v>86</v>
+        <v>75</v>
       </c>
       <c r="AK15" s="2" t="b">
         <v>0</v>
       </c>
       <c r="AL15" t="s">
-        <v>57</v>
+        <v>76</v>
       </c>
     </row>
     <row r="16">
@@ -1519,79 +1537,79 @@
         <v>0</v>
       </c>
       <c r="B16" t="s">
-        <v>54</v>
+        <v>64</v>
       </c>
       <c r="D16" s="2" t="b">
         <v>0</v>
       </c>
       <c r="E16" t="s">
-        <v>59</v>
+        <v>77</v>
       </c>
       <c r="G16" s="2" t="b">
         <v>0</v>
       </c>
       <c r="H16" t="s">
-        <v>87</v>
+        <v>58</v>
       </c>
       <c r="J16" s="2" t="b">
         <v>0</v>
       </c>
       <c r="K16" t="s">
-        <v>59</v>
+        <v>67</v>
       </c>
       <c r="M16" s="2" t="b">
         <v>0</v>
       </c>
       <c r="N16" t="s">
-        <v>88</v>
+        <v>64</v>
       </c>
       <c r="P16" s="2" t="b">
         <v>0</v>
       </c>
       <c r="Q16" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="S16" s="2" t="b">
         <v>0</v>
       </c>
       <c r="T16" t="s">
-        <v>87</v>
+        <v>75</v>
       </c>
       <c r="V16" s="2" t="b">
         <v>0</v>
       </c>
       <c r="W16" t="s">
-        <v>59</v>
+        <v>79</v>
       </c>
       <c r="Y16" s="2" t="b">
         <v>0</v>
       </c>
       <c r="Z16" t="s">
-        <v>89</v>
+        <v>70</v>
       </c>
       <c r="AB16" s="2" t="b">
         <v>0</v>
       </c>
       <c r="AC16" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="AE16" s="2" t="b">
         <v>0</v>
       </c>
       <c r="AF16" t="s">
-        <v>76</v>
+        <v>56</v>
       </c>
       <c r="AH16" s="2" t="b">
         <v>0</v>
       </c>
       <c r="AI16" t="s">
-        <v>72</v>
+        <v>80</v>
       </c>
       <c r="AK16" s="2" t="b">
         <v>0</v>
       </c>
       <c r="AL16" t="s">
-        <v>71</v>
+        <v>81</v>
       </c>
     </row>
     <row r="17">
@@ -1599,31 +1617,31 @@
         <v>0</v>
       </c>
       <c r="B17" t="s">
-        <v>65</v>
+        <v>82</v>
       </c>
       <c r="D17" s="2" t="b">
         <v>0</v>
       </c>
       <c r="E17" t="s">
-        <v>77</v>
+        <v>59</v>
       </c>
       <c r="G17" s="2" t="b">
         <v>0</v>
       </c>
       <c r="H17" t="s">
-        <v>90</v>
+        <v>75</v>
       </c>
       <c r="J17" s="2" t="b">
         <v>0</v>
       </c>
       <c r="K17" t="s">
-        <v>77</v>
+        <v>59</v>
       </c>
       <c r="M17" s="2" t="b">
         <v>0</v>
       </c>
       <c r="N17" t="s">
-        <v>54</v>
+        <v>82</v>
       </c>
       <c r="P17" s="2" t="b">
         <v>0</v>
@@ -1635,37 +1653,37 @@
         <v>0</v>
       </c>
       <c r="T17" t="s">
-        <v>91</v>
+        <v>62</v>
       </c>
       <c r="V17" s="2" t="b">
         <v>0</v>
       </c>
       <c r="W17" t="s">
-        <v>77</v>
+        <v>69</v>
       </c>
       <c r="Y17" s="2" t="b">
         <v>0</v>
       </c>
       <c r="Z17" t="s">
-        <v>92</v>
+        <v>84</v>
       </c>
       <c r="AB17" s="2" t="b">
         <v>0</v>
       </c>
       <c r="AC17" t="s">
-        <v>85</v>
+        <v>76</v>
       </c>
       <c r="AE17" s="2" t="b">
         <v>0</v>
       </c>
       <c r="AF17" t="s">
-        <v>93</v>
+        <v>64</v>
       </c>
       <c r="AH17" s="2" t="b">
         <v>0</v>
       </c>
       <c r="AI17" t="s">
-        <v>87</v>
+        <v>62</v>
       </c>
       <c r="AK17" s="2" t="b">
         <v>0</v>
@@ -1679,79 +1697,79 @@
         <v>0</v>
       </c>
       <c r="B18" t="s">
+        <v>86</v>
+      </c>
+      <c r="D18" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E18" t="s">
+        <v>68</v>
+      </c>
+      <c r="G18" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="H18" t="s">
         <v>62</v>
       </c>
-      <c r="D18" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E18" t="s">
-        <v>82</v>
-      </c>
-      <c r="G18" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="H18" t="s">
-        <v>54</v>
-      </c>
       <c r="J18" s="2" t="b">
         <v>0</v>
       </c>
       <c r="K18" t="s">
-        <v>82</v>
+        <v>68</v>
       </c>
       <c r="M18" s="2" t="b">
         <v>0</v>
       </c>
       <c r="N18" t="s">
-        <v>65</v>
+        <v>86</v>
       </c>
       <c r="P18" s="2" t="b">
         <v>0</v>
       </c>
       <c r="Q18" t="s">
+        <v>63</v>
+      </c>
+      <c r="S18" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="T18" t="s">
+        <v>78</v>
+      </c>
+      <c r="V18" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="W18" t="s">
+        <v>77</v>
+      </c>
+      <c r="Y18" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="Z18" t="s">
+        <v>87</v>
+      </c>
+      <c r="AB18" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="AC18" t="s">
+        <v>88</v>
+      </c>
+      <c r="AE18" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="AF18" t="s">
+        <v>67</v>
+      </c>
+      <c r="AH18" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="AI18" t="s">
         <v>89</v>
       </c>
-      <c r="S18" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="T18" t="s">
-        <v>90</v>
-      </c>
-      <c r="V18" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="W18" t="s">
-        <v>82</v>
-      </c>
-      <c r="Y18" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="Z18" t="s">
-        <v>94</v>
-      </c>
-      <c r="AB18" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="AC18" t="s">
-        <v>95</v>
-      </c>
-      <c r="AE18" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="AF18" t="s">
-        <v>71</v>
-      </c>
-      <c r="AH18" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="AI18" t="s">
-        <v>90</v>
-      </c>
       <c r="AK18" s="2" t="b">
         <v>0</v>
       </c>
       <c r="AL18" t="s">
-        <v>96</v>
+        <v>56</v>
       </c>
     </row>
     <row r="19">
@@ -1759,61 +1777,79 @@
         <v>0</v>
       </c>
       <c r="B19" t="s">
+        <v>90</v>
+      </c>
+      <c r="D19" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E19" t="s">
+        <v>64</v>
+      </c>
+      <c r="G19" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="H19" t="s">
+        <v>78</v>
+      </c>
+      <c r="J19" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="K19" t="s">
+        <v>64</v>
+      </c>
+      <c r="M19" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="N19" t="s">
+        <v>90</v>
+      </c>
+      <c r="P19" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q19" t="s">
+        <v>84</v>
+      </c>
+      <c r="S19" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="T19" t="s">
+        <v>91</v>
+      </c>
+      <c r="V19" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="W19" t="s">
+        <v>64</v>
+      </c>
+      <c r="Y19" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="Z19" t="s">
         <v>88</v>
       </c>
-      <c r="D19" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="E19" t="s">
-        <v>88</v>
-      </c>
-      <c r="G19" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="H19" t="s">
-        <v>62</v>
-      </c>
-      <c r="J19" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="K19" t="s">
-        <v>88</v>
-      </c>
-      <c r="M19" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="N19" t="s">
-        <v>62</v>
-      </c>
-      <c r="P19" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="Q19" t="s">
-        <v>97</v>
-      </c>
-      <c r="S19" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="T19" t="s">
-        <v>98</v>
-      </c>
-      <c r="V19" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="W19" t="s">
-        <v>88</v>
+      <c r="AB19" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="AC19" t="s">
+        <v>77</v>
       </c>
       <c r="AE19" s="2" t="b">
         <v>0</v>
       </c>
       <c r="AF19" t="s">
-        <v>99</v>
+        <v>81</v>
       </c>
       <c r="AH19" s="2" t="b">
         <v>0</v>
       </c>
       <c r="AI19" t="s">
-        <v>60</v>
+        <v>78</v>
+      </c>
+      <c r="AK19" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="AL19" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="20">
@@ -1821,31 +1857,31 @@
         <v>0</v>
       </c>
       <c r="B20" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="D20" s="2" t="b">
         <v>0</v>
       </c>
       <c r="E20" t="s">
-        <v>62</v>
+        <v>82</v>
       </c>
       <c r="G20" s="2" t="b">
         <v>0</v>
       </c>
       <c r="H20" t="s">
-        <v>100</v>
+        <v>91</v>
       </c>
       <c r="J20" s="2" t="b">
         <v>0</v>
       </c>
       <c r="K20" t="s">
-        <v>100</v>
+        <v>82</v>
       </c>
       <c r="M20" s="2" t="b">
         <v>0</v>
       </c>
       <c r="N20" t="s">
-        <v>76</v>
+        <v>92</v>
       </c>
       <c r="P20" s="2" t="b">
         <v>0</v>
@@ -1853,17 +1889,47 @@
       <c r="Q20" t="s">
         <v>93</v>
       </c>
+      <c r="S20" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="T20" t="s">
+        <v>94</v>
+      </c>
       <c r="V20" s="2" t="b">
         <v>0</v>
       </c>
       <c r="W20" t="s">
-        <v>85</v>
+        <v>82</v>
+      </c>
+      <c r="Y20" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="Z20" t="s">
+        <v>93</v>
+      </c>
+      <c r="AB20" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="AC20" t="s">
+        <v>95</v>
       </c>
       <c r="AE20" s="2" t="b">
         <v>0</v>
       </c>
       <c r="AF20" t="s">
-        <v>101</v>
+        <v>96</v>
+      </c>
+      <c r="AH20" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="AI20" t="s">
+        <v>91</v>
+      </c>
+      <c r="AK20" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="AL20" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="21">
@@ -1871,49 +1937,79 @@
         <v>0</v>
       </c>
       <c r="B21" t="s">
-        <v>93</v>
+        <v>67</v>
       </c>
       <c r="D21" s="2" t="b">
         <v>0</v>
       </c>
       <c r="E21" t="s">
-        <v>76</v>
+        <v>86</v>
       </c>
       <c r="G21" s="2" t="b">
         <v>0</v>
       </c>
       <c r="H21" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="J21" s="2" t="b">
         <v>0</v>
       </c>
       <c r="K21" t="s">
-        <v>71</v>
+        <v>86</v>
       </c>
       <c r="M21" s="2" t="b">
         <v>0</v>
       </c>
       <c r="N21" t="s">
-        <v>93</v>
+        <v>70</v>
       </c>
       <c r="P21" s="2" t="b">
         <v>0</v>
       </c>
       <c r="Q21" t="s">
-        <v>101</v>
+        <v>98</v>
+      </c>
+      <c r="S21" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="T21" t="s">
+        <v>97</v>
       </c>
       <c r="V21" s="2" t="b">
         <v>0</v>
       </c>
       <c r="W21" t="s">
-        <v>103</v>
+        <v>86</v>
+      </c>
+      <c r="Y21" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="Z21" t="s">
+        <v>99</v>
+      </c>
+      <c r="AB21" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="AC21" t="s">
+        <v>100</v>
       </c>
       <c r="AE21" s="2" t="b">
         <v>0</v>
       </c>
       <c r="AF21" t="s">
-        <v>104</v>
+        <v>77</v>
+      </c>
+      <c r="AH21" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="AI21" t="s">
+        <v>97</v>
+      </c>
+      <c r="AK21" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="AL21" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="22">
@@ -1921,37 +2017,67 @@
         <v>0</v>
       </c>
       <c r="B22" t="s">
-        <v>71</v>
+        <v>92</v>
       </c>
       <c r="D22" s="2" t="b">
         <v>0</v>
       </c>
       <c r="E22" t="s">
-        <v>93</v>
+        <v>92</v>
+      </c>
+      <c r="G22" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="H22" t="s">
+        <v>67</v>
       </c>
       <c r="J22" s="2" t="b">
         <v>0</v>
       </c>
       <c r="K22" t="s">
-        <v>99</v>
+        <v>92</v>
       </c>
       <c r="M22" s="2" t="b">
         <v>0</v>
       </c>
       <c r="N22" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="P22" s="2" t="b">
         <v>0</v>
       </c>
       <c r="Q22" t="s">
-        <v>104</v>
+        <v>101</v>
+      </c>
+      <c r="S22" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="T22" t="s">
+        <v>102</v>
+      </c>
+      <c r="V22" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="W22" t="s">
+        <v>92</v>
+      </c>
+      <c r="Y22" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="Z22" t="s">
+        <v>95</v>
       </c>
       <c r="AE22" s="2" t="b">
         <v>0</v>
       </c>
       <c r="AF22" t="s">
-        <v>67</v>
+        <v>103</v>
+      </c>
+      <c r="AH22" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="AI22" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="23">
@@ -1959,31 +2085,55 @@
         <v>0</v>
       </c>
       <c r="B23" t="s">
-        <v>99</v>
+        <v>81</v>
       </c>
       <c r="D23" s="2" t="b">
         <v>0</v>
       </c>
       <c r="E23" t="s">
-        <v>99</v>
+        <v>67</v>
+      </c>
+      <c r="G23" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="H23" t="s">
+        <v>104</v>
       </c>
       <c r="J23" s="2" t="b">
         <v>0</v>
       </c>
       <c r="K23" t="s">
+        <v>104</v>
+      </c>
+      <c r="M23" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="N23" t="s">
+        <v>81</v>
+      </c>
+      <c r="P23" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q23" t="s">
+        <v>96</v>
+      </c>
+      <c r="V23" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="W23" t="s">
+        <v>95</v>
+      </c>
+      <c r="Y23" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="Z23" t="s">
+        <v>98</v>
+      </c>
+      <c r="AE23" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="AF23" t="s">
         <v>105</v>
-      </c>
-      <c r="M23" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="N23" t="s">
-        <v>99</v>
-      </c>
-      <c r="P23" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="Q23" t="s">
-        <v>106</v>
       </c>
     </row>
     <row r="24">
@@ -1991,19 +2141,55 @@
         <v>0</v>
       </c>
       <c r="B24" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="D24" s="2" t="b">
         <v>0</v>
       </c>
       <c r="E24" t="s">
-        <v>101</v>
+        <v>81</v>
+      </c>
+      <c r="G24" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="H24" t="s">
+        <v>106</v>
+      </c>
+      <c r="J24" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="K24" t="s">
+        <v>77</v>
       </c>
       <c r="M24" s="2" t="b">
         <v>0</v>
       </c>
       <c r="N24" t="s">
-        <v>101</v>
+        <v>96</v>
+      </c>
+      <c r="P24" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q24" t="s">
+        <v>105</v>
+      </c>
+      <c r="V24" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="W24" t="s">
+        <v>107</v>
+      </c>
+      <c r="Y24" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="Z24" t="s">
+        <v>108</v>
+      </c>
+      <c r="AE24" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="AF24" t="s">
+        <v>109</v>
       </c>
     </row>
     <row r="25">
@@ -2011,19 +2197,43 @@
         <v>0</v>
       </c>
       <c r="B25" t="s">
-        <v>104</v>
+        <v>77</v>
       </c>
       <c r="D25" s="2" t="b">
         <v>0</v>
       </c>
       <c r="E25" t="s">
-        <v>104</v>
+        <v>96</v>
+      </c>
+      <c r="J25" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="K25" t="s">
+        <v>103</v>
       </c>
       <c r="M25" s="2" t="b">
         <v>0</v>
       </c>
       <c r="N25" t="s">
-        <v>104</v>
+        <v>77</v>
+      </c>
+      <c r="P25" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q25" t="s">
+        <v>109</v>
+      </c>
+      <c r="Y25" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="Z25" t="s">
+        <v>110</v>
+      </c>
+      <c r="AE25" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="AF25" t="s">
+        <v>73</v>
       </c>
     </row>
     <row r="26">
@@ -2031,19 +2241,91 @@
         <v>0</v>
       </c>
       <c r="B26" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="D26" s="2" t="b">
         <v>0</v>
       </c>
       <c r="E26" t="s">
-        <v>52</v>
+        <v>103</v>
+      </c>
+      <c r="J26" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="K26" t="s">
+        <v>111</v>
       </c>
       <c r="M26" s="2" t="b">
         <v>0</v>
       </c>
       <c r="N26" t="s">
-        <v>53</v>
+        <v>103</v>
+      </c>
+      <c r="P26" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q26" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="B27" t="s">
+        <v>105</v>
+      </c>
+      <c r="D27" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E27" t="s">
+        <v>105</v>
+      </c>
+      <c r="M27" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="N27" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="B28" t="s">
+        <v>109</v>
+      </c>
+      <c r="D28" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E28" t="s">
+        <v>109</v>
+      </c>
+      <c r="M28" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="N28" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="B29" t="s">
+        <v>113</v>
+      </c>
+      <c r="D29" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E29" t="s">
+        <v>55</v>
+      </c>
+      <c r="M29" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="N29" t="s">
+        <v>61</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add a bunch of builds
</commit_message>
<xml_diff>
--- a/Assets/Exports/Main Characters.xlsx
+++ b/Assets/Exports/Main Characters.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="115">
   <si>
     <t>Ramza</t>
   </si>
@@ -298,7 +298,7 @@
     <t>3 Time Mage</t>
   </si>
   <si>
-    <t>Master Ninja! (1,120 JP)</t>
+    <t>Shuriken: (Ninja - 50 JP)</t>
   </si>
   <si>
     <t>Move-MP Up: (Oracle - 350 JP)</t>
@@ -313,6 +313,9 @@
     <t>3 Oracle</t>
   </si>
   <si>
+    <t>Ball: (Ninja - 70 JP)</t>
+  </si>
+  <si>
     <t>Master Oracle! (4,670 JP)</t>
   </si>
   <si>
@@ -322,13 +325,13 @@
     <t>Damage Split: (Calculator - 300 JP)</t>
   </si>
   <si>
+    <t>2 Oracle</t>
+  </si>
+  <si>
+    <t>Teleport: (Time Mage - 600 JP)</t>
+  </si>
+  <si>
     <t>Master Divine Knight! (1,900 JP)</t>
-  </si>
-  <si>
-    <t>2 Oracle</t>
-  </si>
-  <si>
-    <t>Teleport: (Time Mage - 600 JP)</t>
   </si>
   <si>
     <t>4 Mediator</t>
@@ -1973,7 +1976,7 @@
         <v>0</v>
       </c>
       <c r="T21" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="V21" s="2" t="b">
         <v>0</v>
@@ -1985,13 +1988,13 @@
         <v>0</v>
       </c>
       <c r="Z21" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="AB21" s="2" t="b">
         <v>0</v>
       </c>
       <c r="AC21" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="AE21" s="2" t="b">
         <v>0</v>
@@ -2047,13 +2050,13 @@
         <v>0</v>
       </c>
       <c r="Q22" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="S22" s="2" t="b">
         <v>0</v>
       </c>
       <c r="T22" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="V22" s="2" t="b">
         <v>0</v>
@@ -2117,6 +2120,12 @@
       <c r="Q23" t="s">
         <v>96</v>
       </c>
+      <c r="S23" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="T23" t="s">
+        <v>105</v>
+      </c>
       <c r="V23" s="2" t="b">
         <v>0</v>
       </c>
@@ -2133,7 +2142,7 @@
         <v>0</v>
       </c>
       <c r="AF23" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
     </row>
     <row r="24">
@@ -2153,7 +2162,7 @@
         <v>0</v>
       </c>
       <c r="H24" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="J24" s="2" t="b">
         <v>0</v>
@@ -2171,25 +2180,25 @@
         <v>0</v>
       </c>
       <c r="Q24" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="V24" s="2" t="b">
         <v>0</v>
       </c>
       <c r="W24" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="Y24" s="2" t="b">
         <v>0</v>
       </c>
       <c r="Z24" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="AE24" s="2" t="b">
         <v>0</v>
       </c>
       <c r="AF24" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
     </row>
     <row r="25">
@@ -2221,13 +2230,13 @@
         <v>0</v>
       </c>
       <c r="Q25" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="Y25" s="2" t="b">
         <v>0</v>
       </c>
       <c r="Z25" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="AE25" s="2" t="b">
         <v>0</v>
@@ -2253,7 +2262,7 @@
         <v>0</v>
       </c>
       <c r="K26" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="M26" s="2" t="b">
         <v>0</v>
@@ -2265,7 +2274,7 @@
         <v>0</v>
       </c>
       <c r="Q26" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
     </row>
     <row r="27">
@@ -2273,19 +2282,19 @@
         <v>0</v>
       </c>
       <c r="B27" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="D27" s="2" t="b">
         <v>0</v>
       </c>
       <c r="E27" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="M27" s="2" t="b">
         <v>0</v>
       </c>
       <c r="N27" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
     </row>
     <row r="28">
@@ -2293,19 +2302,19 @@
         <v>0</v>
       </c>
       <c r="B28" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="D28" s="2" t="b">
         <v>0</v>
       </c>
       <c r="E28" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="M28" s="2" t="b">
         <v>0</v>
       </c>
       <c r="N28" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
     </row>
     <row r="29">
@@ -2313,7 +2322,7 @@
         <v>0</v>
       </c>
       <c r="B29" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="D29" s="2" t="b">
         <v>0</v>

</xml_diff>